<commit_message>
wrapped up educator import
</commit_message>
<xml_diff>
--- a/assets/static/educator_example.xlsx
+++ b/assets/static/educator_example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshcrawmer/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshcrawmer/Desktop/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07E18689-9B5C-CD4C-BD61-8562155FB1A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16BF88B-CA94-2349-859A-D3666080A062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{F013B0DF-93E5-ED44-8A85-F2C7596521C4}"/>
   </bookViews>
@@ -44,31 +44,31 @@
     <t>Email</t>
   </si>
   <si>
-    <t>user one first name</t>
-  </si>
-  <si>
-    <t>user one last name</t>
-  </si>
-  <si>
-    <t>user_one@gmail.com</t>
-  </si>
-  <si>
-    <t>user two first name</t>
-  </si>
-  <si>
-    <t>user two last name</t>
-  </si>
-  <si>
-    <t>user_two@gmail.com</t>
-  </si>
-  <si>
-    <t>user three first name</t>
-  </si>
-  <si>
-    <t>user three last name</t>
-  </si>
-  <si>
-    <t>user_three@gmail.com</t>
+    <t>educator one first name</t>
+  </si>
+  <si>
+    <t>educator two first name</t>
+  </si>
+  <si>
+    <t>educator three first name</t>
+  </si>
+  <si>
+    <t>educator one last name</t>
+  </si>
+  <si>
+    <t>educator two last name</t>
+  </si>
+  <si>
+    <t>educator three last name</t>
+  </si>
+  <si>
+    <t>educator1@some-school.org</t>
+  </si>
+  <si>
+    <t>educator2@some-school.org</t>
+  </si>
+  <si>
+    <t>educator3@some-school.org</t>
   </si>
 </sst>
 </file>
@@ -434,7 +434,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -455,29 +455,29 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
@@ -485,9 +485,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{7310F719-B143-2B41-9366-739E8C6B7B36}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{3AB229E1-1C98-3949-BB06-59341D395FE1}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{F68052F7-A878-504E-AE03-391439A6F049}"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{F68052F7-A878-504E-AE03-391439A6F049}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{DCE4F8E1-750E-5040-A28E-C0D1DC6A2EA5}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{FB0748EE-76B2-6C40-802A-5A37D8DA3B7D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>